<commit_message>
event template import latest changes
</commit_message>
<xml_diff>
--- a/reports-api/src/reports_api/templates/configurations/event_configurations.xlsx
+++ b/reports-api/src/reports_api/templates/configurations/event_configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\reports-api\src\reports_api\templates\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB98D7F-B05B-447E-8553-A32C0EFB418C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6070A279-7E72-4E7C-A736-407234E6D148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A853713A-B735-4946-989C-636E29001BC2}"/>
+    <workbookView xWindow="37155" yWindow="5430" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{A853713A-B735-4946-989C-636E29001BC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>Milestone</t>
+  </si>
+  <si>
+    <t>Update/Tweet: PCP Coming Soon</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Early Engagement</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>#54858d</t>
+  </si>
+  <si>
+    <t>Legislated</t>
   </si>
 </sst>
 </file>
@@ -115,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,9 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C810C-8C59-436D-942F-1E4DCF6E7DB1}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,9 +501,10 @@
     <col min="2" max="3" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -490,13 +521,16 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,11 +546,40 @@
       <c r="E2">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -526,22 +589,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153731F1-A4DA-4C0A-A099-407D72EC11B0}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -569,8 +632,11 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -597,6 +663,41 @@
       </c>
       <c r="I2" t="b">
         <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>